<commit_message>
refactor: Refactor and optimize microgrid server codebase.
- Add new solver `scip` with its parameters
- Implement a function to flatten mappings and check for duplicates in `type_utils.py`
- Swap the port definitions for `变压器` and `变流器` in `topo_check.py`
- Rename `solveModelFromCalcParamfList` to `solveModelFromCalcParamList` in multiple files
- Fix commented out code in `mock_utils.py` and `debug_utils.py`
- Add `residualEquipmentAnnualFactor` to `CalculationResult` dictionary in `fastapi_celery_functions.py`
</commit_message>
<xml_diff>
--- a/microgrid_base/sim_param_export.xlsx
+++ b/microgrid_base/sim_param_export.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -441,132 +441,132 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>自来水消耗费用</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗量</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>元件类型</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽产量</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽收入</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>设备维护费用</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>热收入</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗费用</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽负荷</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>产热量</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>产电量</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>冷收入</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>柴油消耗费用</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>柴油消耗量</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>氢气产量</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>自来水消耗量</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>热负荷</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>设备台数</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>氢气收入</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗量</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>自来水消耗费用</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽收入</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗费用</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>氢气产量</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>柴油消耗量</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>热收入</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>氢气消耗量</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>产电量</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>设备台数</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>产热量</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>产冷量</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>电收入</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>电负荷</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽负荷</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>元件类型</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽产量</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>设备型号</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>冷负荷</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>平均效率/平均COP</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>自来水消耗量</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>柴油消耗费用</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>设备维护费用</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>热负荷</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>产冷量</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>冷收入</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>冷负荷</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>设备型号</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>电收入</t>
         </is>
       </c>
     </row>
@@ -578,35 +578,35 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
-      <c r="O2" t="inlineStr"/>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
@@ -623,7 +623,11 @@
       </c>
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -633,32 +637,28 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr"/>
-      <c r="X3" t="inlineStr"/>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="AA3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -668,18 +668,22 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H4" t="inlineStr"/>
       <c r="I4" t="inlineStr"/>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
         <is>
           <t>x</t>
@@ -688,29 +692,25 @@
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z4" t="inlineStr"/>
       <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -721,18 +721,22 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H5" t="inlineStr"/>
       <c r="I5" t="inlineStr"/>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
         <is>
           <t>x</t>
@@ -741,29 +745,25 @@
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z5" t="inlineStr"/>
       <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -774,22 +774,22 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
         <is>
           <t>x</t>
@@ -797,35 +797,35 @@
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S6" t="inlineStr"/>
+      <c r="R6" t="inlineStr"/>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z6" t="inlineStr"/>
+      <c r="AA6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -835,50 +835,50 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z7" t="inlineStr"/>
+      <c r="AA7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -888,50 +888,50 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L8" t="inlineStr"/>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S8" t="inlineStr"/>
+      <c r="R8" t="inlineStr"/>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z8" t="inlineStr"/>
+      <c r="AA8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -941,50 +941,50 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L9" t="inlineStr"/>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S9" t="inlineStr"/>
+      <c r="R9" t="inlineStr"/>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z9" t="inlineStr"/>
+      <c r="AA9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -994,50 +994,50 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="L10" t="inlineStr"/>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S10" t="inlineStr"/>
+      <c r="R10" t="inlineStr"/>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z10" t="inlineStr"/>
+      <c r="AA10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1047,10 +1047,18 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
@@ -1059,34 +1067,26 @@
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="AA11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Z11" t="inlineStr"/>
+      <c r="AA11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
refactor: Refactor topology verification and type checking.
- Refactor and improve readability of `main_parser` function in `lib_parse_params.py`
- Add basic type checking mode for Python analysis in `settings.json`
- Modify various functions in `type_utils.py.j2` to include new dictionary `port_name_to_energy_type`
- Add translation tables and verifiers for device types in `render_type_utils.py`
</commit_message>
<xml_diff>
--- a/microgrid_base/sim_param_export.xlsx
+++ b/microgrid_base/sim_param_export.xlsx
@@ -441,132 +441,132 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>电收入</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽收入</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>热收入</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>产热量</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽产量</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>设备台数</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>氢气收入</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>产电量</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>柴油消耗费用</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>氢气产量</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>设备维护费用</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗量</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>电负荷</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
           <t>自来水消耗费用</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗量</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽负荷</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗费用</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>平均效率/平均COP</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>氢气消耗量</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>元件类型</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽产量</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽收入</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>设备维护费用</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>热收入</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗费用</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽负荷</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>产热量</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>产电量</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>热负荷</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>冷负荷</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>冷收入</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>柴油消耗费用</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>自来水消耗量</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>柴油消耗量</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>氢气产量</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>自来水消耗量</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>热负荷</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>设备台数</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>氢气收入</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>氢气消耗量</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>设备型号</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>产冷量</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>电收入</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>电负荷</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>设备型号</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>冷负荷</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>平均效率/平均COP</t>
         </is>
       </c>
     </row>
@@ -578,40 +578,40 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z2" t="inlineStr"/>
       <c r="AA2" t="inlineStr"/>
     </row>
@@ -621,13 +621,13 @@
           <t>电负荷</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
@@ -637,25 +637,25 @@
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
-      <c r="N3" t="inlineStr"/>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
-      <c r="T3" t="inlineStr"/>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
       <c r="Y3" t="inlineStr"/>
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
@@ -668,11 +668,7 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
@@ -681,7 +677,11 @@
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
       <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr">
@@ -695,22 +695,22 @@
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -721,11 +721,7 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
@@ -734,7 +730,11 @@
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
       <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr">
@@ -748,22 +748,22 @@
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T5" t="inlineStr"/>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -774,11 +774,7 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
@@ -787,7 +783,11 @@
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
       <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr">
@@ -797,20 +797,20 @@
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="O6" t="inlineStr"/>
       <c r="P6" t="inlineStr"/>
       <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T6" t="inlineStr"/>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
@@ -820,12 +820,12 @@
           <t>x</t>
         </is>
       </c>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -835,11 +835,7 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
@@ -851,34 +847,38 @@
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
       <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T7" t="inlineStr"/>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -888,11 +888,7 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
@@ -904,34 +900,38 @@
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
       <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T8" t="inlineStr"/>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U8" t="inlineStr"/>
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -941,11 +941,7 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
@@ -957,34 +953,38 @@
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
       <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T9" t="inlineStr"/>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -994,11 +994,7 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
@@ -1010,34 +1006,38 @@
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
       <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="T10" t="inlineStr"/>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1047,46 +1047,46 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D11" t="inlineStr"/>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
       <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
       <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Y11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA11" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat: Revise and enhance microgrid report template and export method
- Added a new file `microgrid_base/report_template.md.j2`
- Modified and added content in the `report_template.md.j2` file
- Updated and fixed code in the `export_format_validate.py.j2` file
- Modified and fixed code in the `plot_utils.py` file
- Modified and fixed code in the `export_format_validate.py` file
- Modified and updated the `sim_param_export.xlsx` file
</commit_message>
<xml_diff>
--- a/microgrid_base/sim_param_export.xlsx
+++ b/microgrid_base/sim_param_export.xlsx
@@ -441,132 +441,132 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>自来水消耗费用</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>自来水消耗量</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>设备维护费用</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽收入</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>蒸汽负荷</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>氢气产量</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>产冷量</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>产电量</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>电负荷</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>产热量</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>热负荷</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>平均效率/平均COP</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>柴油消耗量</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>冷负荷</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>氢气收入</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>元件类型</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
           <t>蒸汽产量</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>氢气产量</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗费用</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>柴油消耗费用</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>冷收入</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>设备台数</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>天然气消耗量</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>热收入</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>氢气消耗量</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>设备型号</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>电收入</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>冷负荷</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>氢气消耗量</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>自来水消耗费用</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>冷收入</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽收入</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>元件类型</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>产冷量</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>自来水消耗量</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>设备台数</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>氢气收入</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗量</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>设备维护费用</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>产热量</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>设备型号</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>热收入</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>柴油消耗量</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>产电量</t>
-        </is>
-      </c>
-      <c r="W1" s="1" t="inlineStr">
-        <is>
-          <t>天然气消耗费用</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>平均效率/平均COP</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>热负荷</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>蒸汽负荷</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>电负荷</t>
         </is>
       </c>
     </row>
@@ -578,36 +578,36 @@
       </c>
       <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="D2" t="inlineStr"/>
       <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr"/>
       <c r="I2" t="inlineStr"/>
       <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
-      <c r="N2" t="inlineStr"/>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="O2" t="inlineStr"/>
       <c r="P2" t="inlineStr"/>
-      <c r="Q2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
-      <c r="T2" t="inlineStr"/>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
@@ -624,27 +624,27 @@
       <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
       <c r="T3" t="inlineStr"/>
@@ -668,25 +668,25 @@
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E4" t="inlineStr"/>
       <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K4" t="inlineStr"/>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
-      <c r="N4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr"/>
       <c r="P4" t="inlineStr"/>
       <c r="Q4" t="inlineStr">
@@ -695,11 +695,7 @@
         </is>
       </c>
       <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S4" t="inlineStr"/>
       <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr"/>
       <c r="V4" t="inlineStr">
@@ -710,7 +706,11 @@
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
       <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA4" t="inlineStr"/>
     </row>
     <row r="5">
@@ -721,25 +721,25 @@
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E5" t="inlineStr"/>
       <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K5" t="inlineStr"/>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr"/>
       <c r="P5" t="inlineStr"/>
       <c r="Q5" t="inlineStr">
@@ -748,11 +748,7 @@
         </is>
       </c>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S5" t="inlineStr"/>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr">
@@ -763,7 +759,11 @@
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
       <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
+      <c r="Z5" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA5" t="inlineStr"/>
     </row>
     <row r="6">
@@ -774,20 +774,28 @@
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K6" t="inlineStr"/>
       <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr">
         <is>
           <t>x</t>
@@ -801,30 +809,22 @@
         </is>
       </c>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S6" t="inlineStr"/>
       <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
       <c r="W6" t="inlineStr"/>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X6" t="inlineStr"/>
       <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
+      <c r="Z6" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA6" t="inlineStr"/>
     </row>
     <row r="7">
@@ -835,25 +835,25 @@
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E7" t="inlineStr"/>
       <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr"/>
       <c r="I7" t="inlineStr"/>
       <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr">
@@ -862,22 +862,22 @@
         </is>
       </c>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S7" t="inlineStr"/>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
-      <c r="V7" t="inlineStr"/>
+      <c r="V7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W7" t="inlineStr"/>
-      <c r="X7" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X7" t="inlineStr"/>
       <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
+      <c r="Z7" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA7" t="inlineStr"/>
     </row>
     <row r="8">
@@ -888,25 +888,25 @@
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E8" t="inlineStr"/>
       <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K8" t="inlineStr"/>
       <c r="L8" t="inlineStr"/>
-      <c r="M8" t="inlineStr"/>
-      <c r="N8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
       <c r="Q8" t="inlineStr">
@@ -915,22 +915,22 @@
         </is>
       </c>
       <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S8" t="inlineStr"/>
       <c r="T8" t="inlineStr"/>
       <c r="U8" t="inlineStr"/>
-      <c r="V8" t="inlineStr"/>
+      <c r="V8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W8" t="inlineStr"/>
-      <c r="X8" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X8" t="inlineStr"/>
       <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
+      <c r="Z8" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA8" t="inlineStr"/>
     </row>
     <row r="9">
@@ -941,25 +941,25 @@
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E9" t="inlineStr"/>
       <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K9" t="inlineStr"/>
       <c r="L9" t="inlineStr"/>
-      <c r="M9" t="inlineStr"/>
-      <c r="N9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr"/>
       <c r="P9" t="inlineStr"/>
       <c r="Q9" t="inlineStr">
@@ -968,22 +968,22 @@
         </is>
       </c>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S9" t="inlineStr"/>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
-      <c r="V9" t="inlineStr"/>
+      <c r="V9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W9" t="inlineStr"/>
-      <c r="X9" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X9" t="inlineStr"/>
       <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
+      <c r="Z9" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -994,25 +994,25 @@
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E10" t="inlineStr"/>
       <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K10" t="inlineStr"/>
       <c r="L10" t="inlineStr"/>
-      <c r="M10" t="inlineStr"/>
-      <c r="N10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
       <c r="Q10" t="inlineStr">
@@ -1021,22 +1021,22 @@
         </is>
       </c>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S10" t="inlineStr"/>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
-      <c r="V10" t="inlineStr"/>
+      <c r="V10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W10" t="inlineStr"/>
-      <c r="X10" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X10" t="inlineStr"/>
       <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
+      <c r="Z10" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA10" t="inlineStr"/>
     </row>
     <row r="11">
@@ -1047,20 +1047,24 @@
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E11" t="inlineStr"/>
       <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr"/>
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr"/>
       <c r="P11" t="inlineStr"/>
@@ -1070,22 +1074,18 @@
         </is>
       </c>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="S11" t="inlineStr"/>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="X11" t="inlineStr"/>
       <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
+      <c r="Z11" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA11" t="inlineStr"/>
     </row>
     <row r="12">
@@ -1099,29 +1099,25 @@
       <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr"/>
       <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="G12" t="inlineStr"/>
       <c r="H12" t="inlineStr"/>
       <c r="I12" t="inlineStr"/>
       <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="K12" t="inlineStr"/>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
       <c r="T12" t="inlineStr"/>
@@ -1129,7 +1125,11 @@
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="Z12" t="inlineStr"/>
       <c r="AA12" t="inlineStr"/>
     </row>
@@ -1141,12 +1141,20 @@
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="J13" t="inlineStr"/>
       <c r="K13" t="inlineStr">
         <is>
@@ -1155,32 +1163,16 @@
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="P13" t="inlineStr"/>
       <c r="Q13" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="R13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S13" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="R13" t="inlineStr"/>
+      <c r="S13" t="inlineStr"/>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr">
@@ -1188,10 +1180,18 @@
           <t>x</t>
         </is>
       </c>
-      <c r="W13" t="inlineStr"/>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="X13" t="inlineStr"/>
       <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="AA13" t="inlineStr"/>
     </row>
     <row r="14">
@@ -1201,18 +1201,26 @@
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="E14" t="inlineStr"/>
       <c r="F14" t="inlineStr"/>
-      <c r="G14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="H14" t="inlineStr"/>
       <c r="I14" t="inlineStr"/>
-      <c r="J14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="K14" t="inlineStr">
         <is>
           <t>x</t>
@@ -1220,11 +1228,7 @@
       </c>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="inlineStr"/>
-      <c r="N14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr">
@@ -1232,28 +1236,24 @@
           <t>x</t>
         </is>
       </c>
-      <c r="R14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
-      <c r="S14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
-      <c r="V14" t="inlineStr"/>
+      <c r="V14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
       <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr">
-        <is>
-          <t>x</t>
-        </is>
-      </c>
+      <c r="Z14" t="inlineStr">
+        <is>
+          <t>x</t>
+        </is>
+      </c>
+      <c r="AA14" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>